<commit_message>
Lab 1 protocol updated.
</commit_message>
<xml_diff>
--- a/cp1/bila_fb-02_leta_fb-02_cp1/frequency_of_bigrams.xlsx
+++ b/cp1/bila_fb-02_leta_fb-02_cp1/frequency_of_bigrams.xlsx
@@ -607,103 +607,103 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.003422027875427515</v>
+        <v>0.0001787456030788379</v>
       </c>
       <c r="C2" t="n">
-        <v>0.001053664485028628</v>
+        <v>0.0002405342066122633</v>
       </c>
       <c r="D2" t="n">
-        <v>0.001583354768641573</v>
+        <v>0.006013355165306582</v>
       </c>
       <c r="E2" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.001237978806508988</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.00368745558944121</v>
       </c>
       <c r="G2" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.0007171891481558308</v>
       </c>
       <c r="H2" t="n">
-        <v>8.193051149408862e-05</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.00114512180018482</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>0.001107781391920699</v>
       </c>
       <c r="K2" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.003464575269552783</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>0.0009996513357372042</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0008421694437299341</v>
+        <v>6.399533937390491e-05</v>
       </c>
       <c r="N2" t="n">
-        <v>0.004860575228405118</v>
+        <v>0.0001809523389193173</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0009450589232806501</v>
+        <v>0.005702205411798975</v>
       </c>
       <c r="P2" t="n">
-        <v>1.714824659178599e-05</v>
+        <v>0.002275144651534344</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.002142740501105575</v>
       </c>
       <c r="R2" t="n">
-        <v>0.004837710899616069</v>
+        <v>0.009914864131274301</v>
       </c>
       <c r="S2" t="n">
-        <v>0.0004401383291891737</v>
+        <v>0.0002295005274098659</v>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>0.001176190202975563</v>
       </c>
       <c r="U2" t="n">
-        <v>0.00466622843369821</v>
+        <v>0.009934724753838617</v>
       </c>
       <c r="V2" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0.0016131238993905</v>
       </c>
       <c r="W2" t="n">
-        <v>0</v>
+        <v>0.006664342238248028</v>
       </c>
       <c r="X2" t="n">
-        <v>0.0002972362742576238</v>
+        <v>0.0003927989796053473</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.006945039869673326</v>
+        <v>0.000428106753053019</v>
       </c>
       <c r="Z2" t="n">
-        <v>8.193051149408862e-05</v>
+        <v>0.0007878046950511742</v>
       </c>
       <c r="AA2" t="n">
-        <v>0</v>
+        <v>0.0001632984521954815</v>
       </c>
       <c r="AB2" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.002200115632958041</v>
       </c>
       <c r="AC2" t="n">
-        <v>0</v>
+        <v>0.0003861787720839089</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.005599855192584336</v>
+        <v>0.0004501741114578138</v>
       </c>
       <c r="AE2" t="n">
         <v>0</v>
       </c>
       <c r="AF2" t="n">
-        <v>0</v>
+        <v>7.282228273582282e-05</v>
       </c>
       <c r="AG2" t="n">
-        <v>0</v>
+        <v>3.751450928815116e-05</v>
       </c>
       <c r="AH2" t="n">
-        <v>4.95393790429373e-05</v>
+        <v>0.0001213704712263714</v>
       </c>
     </row>
     <row r="3">
@@ -713,79 +713,79 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.001608124458163042</v>
+        <v>0.0009444829397252173</v>
       </c>
       <c r="C3" t="n">
-        <v>0.008692255661303076</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="D3" t="n">
-        <v>0.001389007973934665</v>
+        <v>0.0001213704712263714</v>
       </c>
       <c r="E3" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>8.826943361917918e-06</v>
       </c>
       <c r="F3" t="n">
-        <v>5.906618270504063e-05</v>
+        <v>3.530777344767167e-05</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.001853658106002763</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>8.826943361917918e-06</v>
       </c>
       <c r="I3" t="n">
-        <v>0.000621147598769137</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>0.000110336792023974</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>0.0008186989968178869</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>0.0002559813574956197</v>
       </c>
       <c r="N3" t="n">
-        <v>1.905360732420665e-05</v>
+        <v>0.0001279906787478098</v>
       </c>
       <c r="O3" t="n">
-        <v>0.001701487134051654</v>
+        <v>0.000216260112366989</v>
       </c>
       <c r="P3" t="n">
-        <v>0.00185963207484257</v>
+        <v>1.10336792023974e-05</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.0009183838730267607</v>
+        <v>0.0002008129614836326</v>
       </c>
       <c r="R3" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>6.178860353342542e-05</v>
       </c>
       <c r="S3" t="n">
-        <v>0.003728790953347242</v>
+        <v>0.006898256237338853</v>
       </c>
       <c r="T3" t="n">
-        <v>0.004647174826374004</v>
+        <v>1.10336792023974e-05</v>
       </c>
       <c r="U3" t="n">
-        <v>0.004561433593415073</v>
+        <v>4.854818849054855e-05</v>
       </c>
       <c r="V3" t="n">
-        <v>0.0004191793611325464</v>
+        <v>9.268290530013814e-05</v>
       </c>
       <c r="W3" t="n">
-        <v>0.0002191164842283765</v>
+        <v>0.0002979093384647297</v>
       </c>
       <c r="X3" t="n">
-        <v>0</v>
+        <v>0.0004413471680958959</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.0007469014071089009</v>
+        <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>1.905360732420665e-05</v>
+        <v>8.385596193822023e-05</v>
       </c>
       <c r="AA3" t="n">
         <v>0</v>
@@ -797,19 +797,19 @@
         <v>0</v>
       </c>
       <c r="AD3" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.001865348157039832</v>
+        <v>0</v>
       </c>
       <c r="AF3" t="n">
-        <v>0</v>
+        <v>0.0001279906787478098</v>
       </c>
       <c r="AG3" t="n">
-        <v>0</v>
+        <v>0.0001037165845025355</v>
       </c>
       <c r="AH3" t="n">
-        <v>2.095896805662732e-05</v>
+        <v>0.0001699186597169199</v>
       </c>
     </row>
     <row r="4">
@@ -819,103 +819,103 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.002646546057332304</v>
+        <v>0.003844133834115253</v>
       </c>
       <c r="C4" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>1.765388672383584e-05</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0002419808130174245</v>
+        <v>0.0003530777344767167</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0001467127763963913</v>
+        <v>3.751450928815116e-05</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.001037165845025355</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.002948199082880585</v>
       </c>
       <c r="H4" t="n">
-        <v>4.001257538083398e-05</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0005373117265426277</v>
+        <v>6.178860353342542e-05</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>0.002226596463043795</v>
       </c>
       <c r="L4" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0.005428570167579519</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>0.001586643069304746</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0002972362742576238</v>
+        <v>0.000750290185763023</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>0.0004523808472982933</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0001181323654100813</v>
+        <v>7.502901857630231e-05</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.0006821191422065983</v>
+        <v>0.000856213506106038</v>
       </c>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>0.000161091716355002</v>
       </c>
       <c r="S4" t="n">
-        <v>0.0001638610229881772</v>
+        <v>0.01241068236685659</v>
       </c>
       <c r="T4" t="n">
-        <v>0.01472272237941448</v>
+        <v>2.648083008575376e-05</v>
       </c>
       <c r="U4" t="n">
-        <v>0.003422027875427515</v>
+        <v>0.0008915212795537098</v>
       </c>
       <c r="V4" t="n">
-        <v>0</v>
+        <v>0.002601741555925307</v>
       </c>
       <c r="W4" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>0.007445526725777764</v>
       </c>
       <c r="X4" t="n">
-        <v>0.00306191469700001</v>
+        <v>0.00101951195830152</v>
       </c>
       <c r="Y4" t="n">
         <v>0</v>
       </c>
       <c r="Z4" t="n">
-        <v>0</v>
+        <v>0.0007171891481558308</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.000586851105585565</v>
+        <v>5.296166017150751e-05</v>
       </c>
       <c r="AB4" t="n">
-        <v>0</v>
+        <v>1.544715088335636e-05</v>
       </c>
       <c r="AC4" t="n">
-        <v>0</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="AD4" t="n">
-        <v>0</v>
+        <v>6.620207521438439e-06</v>
       </c>
       <c r="AE4" t="n">
         <v>0</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.002917107281336039</v>
+        <v>0.0007767710158487768</v>
       </c>
       <c r="AG4" t="n">
-        <v>0</v>
+        <v>0.0002515678858146607</v>
       </c>
       <c r="AH4" t="n">
-        <v>9.526803662103327e-06</v>
+        <v>0.002409755537803592</v>
       </c>
     </row>
     <row r="5">
@@ -925,85 +925,85 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.01307839606733545</v>
+        <v>0.0005229963941936367</v>
       </c>
       <c r="C5" t="n">
-        <v>0.000701172749530805</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0001886307125096459</v>
+        <v>6.620207521438439e-05</v>
       </c>
       <c r="E5" t="n">
-        <v>0.006752598435698838</v>
+        <v>8.826943361917918e-06</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0006954566673335429</v>
+        <v>8.164922609774074e-05</v>
       </c>
       <c r="G5" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.002782693894844624</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0002858041098630998</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>8.826943361917918e-06</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>0.0002250870557289069</v>
       </c>
       <c r="L5" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.001134262222006453</v>
       </c>
       <c r="M5" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.0001125435278644535</v>
       </c>
       <c r="N5" t="n">
-        <v>0.003770708889460497</v>
+        <v>0.0001390243579502072</v>
       </c>
       <c r="O5" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>1.544715088335636e-05</v>
       </c>
       <c r="P5" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>3.530777344767167e-05</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.002101612887859994</v>
+        <v>9.930311282157658e-05</v>
       </c>
       <c r="R5" t="n">
-        <v>0.0001467127763963913</v>
+        <v>9.268290530013814e-05</v>
       </c>
       <c r="S5" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0.006790126181155359</v>
       </c>
       <c r="T5" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>0.000638295845360923</v>
+        <v>0.0008473865627441202</v>
       </c>
       <c r="V5" t="n">
-        <v>8.383587222650928e-05</v>
+        <v>3.972124512863063e-05</v>
       </c>
       <c r="W5" t="n">
-        <v>0.0009088570693646575</v>
+        <v>8.826943361917918e-05</v>
       </c>
       <c r="X5" t="n">
-        <v>0.003696399820896091</v>
+        <v>0.001085714033515904</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.0003601131784275058</v>
+        <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>0</v>
+        <v>6.399533937390491e-05</v>
       </c>
       <c r="AA5" t="n">
-        <v>0</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.0004744348223727457</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AC5" t="n">
         <v>0</v>
@@ -1015,13 +1015,13 @@
         <v>0</v>
       </c>
       <c r="AF5" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>6.620207521438439e-05</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.0005144473977535797</v>
+        <v>1.765388672383584e-05</v>
       </c>
       <c r="AH5" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>0.0001169569995454124</v>
       </c>
     </row>
     <row r="6">
@@ -1031,88 +1031,88 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.001196566539960178</v>
+        <v>0.001977235313069614</v>
       </c>
       <c r="C6" t="n">
-        <v>0.002415997408709404</v>
+        <v>1.986062256431532e-05</v>
       </c>
       <c r="D6" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.0005031357716293214</v>
       </c>
       <c r="E6" t="n">
-        <v>0.005134947173873694</v>
+        <v>0.000598025412769939</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0002286432878904799</v>
+        <v>7.282228273582282e-05</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.00610383133476624</v>
       </c>
       <c r="H6" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>0.001094540976877822</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>0.001438791767992621</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>0.001884552407769476</v>
       </c>
       <c r="M6" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.0003685248853600731</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0002877094705955205</v>
+        <v>0.0006708476955057618</v>
       </c>
       <c r="O6" t="n">
-        <v>0.002823744605447426</v>
+        <v>0.0002030196973241121</v>
       </c>
       <c r="P6" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>5.516839601198699e-05</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.0006344851238960816</v>
+        <v>0.0004303134888934985</v>
       </c>
       <c r="R6" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.0003486642627957578</v>
       </c>
       <c r="S6" t="n">
-        <v>0.0002191164842283765</v>
+        <v>0.005823575883025347</v>
       </c>
       <c r="T6" t="n">
-        <v>1.333752512694466e-05</v>
+        <v>6.620207521438439e-06</v>
       </c>
       <c r="U6" t="n">
-        <v>0.00243314565530119</v>
+        <v>5.516839601198699e-05</v>
       </c>
       <c r="V6" t="n">
-        <v>0.00701363285604047</v>
+        <v>0.0004038326588077448</v>
       </c>
       <c r="W6" t="n">
-        <v>0.0004992045118942144</v>
+        <v>0.0007105689406343924</v>
       </c>
       <c r="X6" t="n">
-        <v>0.0006059047129097717</v>
+        <v>0.001308594353404331</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.0001981575161717492</v>
+        <v>0</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.0007297531605171149</v>
+        <v>0.0003883855079243884</v>
       </c>
       <c r="AA6" t="n">
-        <v>0</v>
+        <v>6.620207521438439e-06</v>
       </c>
       <c r="AB6" t="n">
-        <v>0</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.002379795554793411</v>
+        <v>0</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
@@ -1121,13 +1121,13 @@
         <v>0</v>
       </c>
       <c r="AF6" t="n">
-        <v>0</v>
+        <v>0.0002758419800599349</v>
       </c>
       <c r="AG6" t="n">
-        <v>0</v>
+        <v>0.0005605109034817878</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.0001371859727342879</v>
+        <v>0.000856213506106038</v>
       </c>
     </row>
     <row r="7">
@@ -1137,103 +1137,103 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.006537292672935303</v>
+        <v>0.003528570608926688</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0003925043108786571</v>
+        <v>0.001884552407769476</v>
       </c>
       <c r="D7" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0.006050869674594733</v>
       </c>
       <c r="E7" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.0004303134888934985</v>
       </c>
       <c r="F7" t="n">
-        <v>0.001185134375565654</v>
+        <v>0.007231473349251254</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0006916459458687016</v>
+        <v>0.002136120293584136</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0002191164842283765</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0001505234978612326</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>0.003396166458497919</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>0.0002317072632503453</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>0.006119278485649597</v>
       </c>
       <c r="M7" t="n">
-        <v>2.095896805662732e-05</v>
+        <v>0.002411962273644071</v>
       </c>
       <c r="N7" t="n">
-        <v>0.003147655929958939</v>
+        <v>0.0001743321313978789</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>0.0003883855079243884</v>
       </c>
       <c r="P7" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.006019975372828021</v>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>0.005508012657836781</v>
       </c>
       <c r="R7" t="n">
-        <v>0.001009841188182953</v>
+        <v>0.007348430348796667</v>
       </c>
       <c r="S7" t="n">
-        <v>1.714824659178599e-05</v>
+        <v>0.003058535874904559</v>
       </c>
       <c r="T7" t="n">
-        <v>0.0004229900825973877</v>
+        <v>0.003334377854964494</v>
       </c>
       <c r="U7" t="n">
-        <v>0.005956157649547001</v>
+        <v>0.009232982756566142</v>
       </c>
       <c r="V7" t="n">
-        <v>0.0001429020549315499</v>
+        <v>0.00207653842589119</v>
       </c>
       <c r="W7" t="n">
-        <v>0.006735450189107053</v>
+        <v>0.008222297741626541</v>
       </c>
       <c r="X7" t="n">
-        <v>0.0009126677908294988</v>
+        <v>0.001304180881723372</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.0001162270046776606</v>
+        <v>0.0004214865455315806</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.0005220688406832624</v>
+        <v>0.0001809523389193173</v>
       </c>
       <c r="AA7" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.001847037898481324</v>
       </c>
       <c r="AB7" t="n">
-        <v>0</v>
+        <v>0.006640068144002754</v>
       </c>
       <c r="AC7" t="n">
-        <v>4.572865757809597e-05</v>
+        <v>0.002270731179853385</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.00157382796497947</v>
+        <v>0.00339395972265744</v>
       </c>
       <c r="AE7" t="n">
-        <v>0</v>
+        <v>0.0005516839601198699</v>
       </c>
       <c r="AF7" t="n">
-        <v>0</v>
+        <v>0.0003927989796053473</v>
       </c>
       <c r="AG7" t="n">
-        <v>0</v>
+        <v>5.075492433102803e-05</v>
       </c>
       <c r="AH7" t="n">
-        <v>0</v>
+        <v>0.001438791767992621</v>
       </c>
     </row>
     <row r="8">
@@ -1243,28 +1243,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.002779921308601751</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.001286118494383949</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="E8" t="n">
-        <v>3.620185391599265e-05</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.003265788295369021</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0.01626796993340764</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0009564910876751742</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -1279,58 +1279,58 @@
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0003410595711032991</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>0.0002076843198338525</v>
+        <v>1.544715088335636e-05</v>
       </c>
       <c r="P8" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="S8" t="n">
-        <v>0.001495708174950222</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="T8" t="n">
-        <v>0.001379481170272562</v>
+        <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>0.00787295054636219</v>
+        <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>0.008492192784398906</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="W8" t="n">
-        <v>4.191793611325464e-05</v>
+        <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>0.004559528232682653</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.002374079472596149</v>
+        <v>0</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.0003467756533005611</v>
+        <v>0</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.0001581449407909152</v>
+        <v>0</v>
       </c>
       <c r="AB8" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AC8" t="n">
-        <v>0</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="AD8" t="n">
         <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.0009393428410833881</v>
+        <v>0</v>
       </c>
       <c r="AF8" t="n">
         <v>0</v>
@@ -1339,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="AH8" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1349,88 +1349,88 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>0.0003883855079243884</v>
       </c>
       <c r="C9" t="n">
-        <v>0.00286375718082826</v>
+        <v>6.399533937390491e-05</v>
       </c>
       <c r="D9" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.0003641114136791142</v>
       </c>
       <c r="E9" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="F9" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>1.986062256431532e-05</v>
       </c>
       <c r="G9" t="n">
-        <v>1.524288585936533e-05</v>
+        <v>0.0005119627149912393</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0004515704935836977</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>6.620207521438439e-05</v>
       </c>
       <c r="L9" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.0005494772242793905</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>0.0001015098486620561</v>
       </c>
       <c r="N9" t="n">
-        <v>0.0001047948402831366</v>
+        <v>0.0002339139990908248</v>
       </c>
       <c r="O9" t="n">
-        <v>0.0002381700915525832</v>
+        <v>0.0001169569995454124</v>
       </c>
       <c r="P9" t="n">
-        <v>8.193051149408862e-05</v>
+        <v>3.089430176671271e-05</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.0006478226490230262</v>
+        <v>0.000262601565017058</v>
       </c>
       <c r="R9" t="n">
-        <v>0</v>
+        <v>2.20673584047948e-05</v>
       </c>
       <c r="S9" t="n">
-        <v>0</v>
+        <v>0.0007171891481558308</v>
       </c>
       <c r="T9" t="n">
-        <v>0.001177512932635971</v>
+        <v>8.826943361917918e-06</v>
       </c>
       <c r="U9" t="n">
-        <v>0.007474730153286271</v>
+        <v>1.765388672383584e-05</v>
       </c>
       <c r="V9" t="n">
-        <v>0.0009984090237884287</v>
+        <v>0.0001257839429073303</v>
       </c>
       <c r="W9" t="n">
-        <v>2.286432878904799e-05</v>
+        <v>0.000161091716355002</v>
       </c>
       <c r="X9" t="n">
-        <v>0.002395038440652777</v>
+        <v>0.000110336792023974</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.01161888974630122</v>
+        <v>4.192798096911011e-05</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.0004896777082321111</v>
+        <v>0.000267015036698017</v>
       </c>
       <c r="AA9" t="n">
-        <v>9.526803662103327e-06</v>
+        <v>6.620207521438439e-06</v>
       </c>
       <c r="AB9" t="n">
-        <v>1.714824659178599e-05</v>
+        <v>0</v>
       </c>
       <c r="AC9" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0</v>
       </c>
       <c r="AD9" t="n">
         <v>0</v>
@@ -1439,13 +1439,13 @@
         <v>0</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.001509045700077167</v>
+        <v>0.0001699186597169199</v>
       </c>
       <c r="AG9" t="n">
-        <v>0</v>
+        <v>4.854818849054855e-05</v>
       </c>
       <c r="AH9" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.0003619046778386346</v>
       </c>
     </row>
     <row r="10">
@@ -1455,103 +1455,103 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.003742128478474187</v>
+        <v>0.001710220276371597</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="D10" t="n">
-        <v>0.001571922604247049</v>
+        <v>3.972124512863063e-05</v>
       </c>
       <c r="E10" t="n">
-        <v>7.049834709956463e-05</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="F10" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>1.544715088335636e-05</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0007621442929682663</v>
+        <v>0.00110116118439926</v>
       </c>
       <c r="H10" t="n">
-        <v>0.001270875608524584</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>2.286432878904799e-05</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>2.20673584047948e-05</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>0.0006686409596652823</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0001600503015233359</v>
+        <v>4.413471680958959e-05</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>0.0001897792822812353</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>0.0003927989796053473</v>
       </c>
       <c r="P10" t="n">
-        <v>0.0002858041098630998</v>
+        <v>0.0002868756592623324</v>
       </c>
       <c r="Q10" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.0001081300561834945</v>
       </c>
       <c r="R10" t="n">
-        <v>0</v>
+        <v>6.620207521438439e-06</v>
       </c>
       <c r="S10" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.002438443103729825</v>
       </c>
       <c r="T10" t="n">
-        <v>2.476968952146865e-05</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="U10" t="n">
-        <v>1.524288585936533e-05</v>
+        <v>0.0004943088282674034</v>
       </c>
       <c r="V10" t="n">
-        <v>0.0001200377261425019</v>
+        <v>3.31010376071922e-05</v>
       </c>
       <c r="W10" t="n">
-        <v>0.0001028894795507159</v>
+        <v>6.399533937390491e-05</v>
       </c>
       <c r="X10" t="n">
-        <v>0.0009069517086322368</v>
+        <v>0.001118815071123096</v>
       </c>
       <c r="Y10" t="n">
-        <v>2.286432878904799e-05</v>
+        <v>0</v>
       </c>
       <c r="Z10" t="n">
-        <v>0</v>
+        <v>0.0001434378296311662</v>
       </c>
       <c r="AA10" t="n">
-        <v>2.286432878904799e-05</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AB10" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="AC10" t="n">
         <v>0</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.0002248325664256385</v>
+        <v>0</v>
       </c>
       <c r="AE10" t="n">
         <v>0</v>
       </c>
       <c r="AF10" t="n">
-        <v>0</v>
+        <v>6.840881105486387e-05</v>
       </c>
       <c r="AG10" t="n">
-        <v>0</v>
+        <v>3.972124512863063e-05</v>
       </c>
       <c r="AH10" t="n">
-        <v>0.0001009841188182953</v>
+        <v>0.0002250870557289069</v>
       </c>
     </row>
     <row r="11">
@@ -1561,103 +1561,103 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.001590976211571256</v>
+        <v>0.004691520396859374</v>
       </c>
       <c r="C11" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>1.324041504287688e-05</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.0005914052052485005</v>
       </c>
       <c r="E11" t="n">
-        <v>0.005228309849762306</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0004839616260348491</v>
+        <v>3.530777344767167e-05</v>
       </c>
       <c r="G11" t="n">
-        <v>5.906618270504063e-05</v>
+        <v>0.00173890784229783</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0006764030600093363</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>1.714824659178599e-05</v>
+        <v>2.427409424527428e-05</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>0.004578976868994921</v>
       </c>
       <c r="M11" t="n">
-        <v>9.526803662103327e-06</v>
+        <v>0.000267015036698017</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>0.0002030196973241121</v>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>7.944249025726126e-05</v>
       </c>
       <c r="P11" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>1.765388672383584e-05</v>
       </c>
       <c r="Q11" t="n">
-        <v>1.524288585936533e-05</v>
+        <v>0.0001897792822812353</v>
       </c>
       <c r="R11" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>2.20673584047948e-05</v>
       </c>
       <c r="S11" t="n">
-        <v>0</v>
+        <v>0.00334982500584785</v>
       </c>
       <c r="T11" t="n">
-        <v>0</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="U11" t="n">
-        <v>0.0001105109224803986</v>
+        <v>3.31010376071922e-05</v>
       </c>
       <c r="V11" t="n">
-        <v>0.0003963150323434984</v>
+        <v>5.737513185246647e-05</v>
       </c>
       <c r="W11" t="n">
-        <v>0.0004020311145407604</v>
+        <v>0.0001699186597169199</v>
       </c>
       <c r="X11" t="n">
-        <v>0.00205969495174674</v>
+        <v>0.0001787456030788379</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.002810407080320482</v>
+        <v>0</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.0007145102746577496</v>
+        <v>0.0002030196973241121</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.0008154943934760449</v>
+        <v>0</v>
       </c>
       <c r="AB11" t="n">
-        <v>8.955195442377128e-05</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AC11" t="n">
         <v>0</v>
       </c>
       <c r="AD11" t="n">
-        <v>2.095896805662732e-05</v>
+        <v>0</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.0003905989501462365</v>
+        <v>0</v>
       </c>
       <c r="AF11" t="n">
-        <v>0</v>
+        <v>0.0003089430176671271</v>
       </c>
       <c r="AG11" t="n">
-        <v>0</v>
+        <v>6.178860353342542e-05</v>
       </c>
       <c r="AH11" t="n">
-        <v>2.476968952146865e-05</v>
+        <v>0.001160743052092206</v>
       </c>
     </row>
     <row r="12">
@@ -1667,103 +1667,103 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.00300475387502739</v>
+        <v>0.00123135859898755</v>
       </c>
       <c r="C12" t="n">
-        <v>0.001417588384920975</v>
+        <v>0.0004082461304887037</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.006280370202004599</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.001710220276371597</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0003524917354978232</v>
+        <v>0.002526712537349004</v>
       </c>
       <c r="G12" t="n">
-        <v>5.144473977535797e-05</v>
+        <v>0.0015270612016118</v>
       </c>
       <c r="H12" t="n">
-        <v>0.002194975563748607</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>0.002197908897117562</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0009393428410833881</v>
+        <v>0.0008231124684988459</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0008593176903217202</v>
+        <v>0.004038326588077448</v>
       </c>
       <c r="M12" t="n">
-        <v>9.907875808587461e-05</v>
+        <v>0.0003596979419981552</v>
       </c>
       <c r="N12" t="n">
-        <v>0.0008078729505463622</v>
+        <v>0.0007723575441678179</v>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>0.003517536929724291</v>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>0.004996049942845542</v>
       </c>
       <c r="Q12" t="n">
-        <v>0</v>
+        <v>0.004309755096456424</v>
       </c>
       <c r="R12" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.01484691873474594</v>
       </c>
       <c r="S12" t="n">
-        <v>9.526803662103327e-06</v>
+        <v>0.002506851914784689</v>
       </c>
       <c r="T12" t="n">
-        <v>0.0004134632789352844</v>
+        <v>0.0007635306008058999</v>
       </c>
       <c r="U12" t="n">
-        <v>0.0001924414339744872</v>
+        <v>0.005591868619775001</v>
       </c>
       <c r="V12" t="n">
-        <v>0</v>
+        <v>0.002701044668746883</v>
       </c>
       <c r="W12" t="n">
-        <v>0.00249030647727381</v>
+        <v>0.008727640249096341</v>
       </c>
       <c r="X12" t="n">
-        <v>0.0148256118589652</v>
+        <v>0.0004016259229672653</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.00306191469700001</v>
+        <v>0.0006730544313462412</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.0004268008040622291</v>
+        <v>0.001242392278189947</v>
       </c>
       <c r="AA12" t="n">
-        <v>0</v>
+        <v>0.00284227576253757</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.002008250211971381</v>
+        <v>0.001886759143609955</v>
       </c>
       <c r="AC12" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.001052612995908712</v>
       </c>
       <c r="AD12" t="n">
-        <v>0</v>
+        <v>0.001710220276371597</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.0001429020549315499</v>
+        <v>0</v>
       </c>
       <c r="AF12" t="n">
-        <v>0</v>
+        <v>0.0005318233375555545</v>
       </c>
       <c r="AG12" t="n">
-        <v>0</v>
+        <v>0.0002008129614836326</v>
       </c>
       <c r="AH12" t="n">
-        <v>0</v>
+        <v>0.001240185542349468</v>
       </c>
     </row>
     <row r="13">
@@ -1773,94 +1773,94 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.01026608362628255</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.003829775072165538</v>
+        <v>0.00194854774714338</v>
       </c>
       <c r="D13" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.002992333799690174</v>
       </c>
       <c r="E13" t="n">
-        <v>1.524288585936533e-05</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>0.0004170730738506216</v>
       </c>
       <c r="G13" t="n">
-        <v>0.006163841969380853</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>0.004458544113864357</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>5.144473977535797e-05</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.000754703657443982</v>
       </c>
       <c r="L13" t="n">
-        <v>0.003000943153562548</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>0.01490944773119171</v>
+        <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>0.006026655996646565</v>
+        <v>0</v>
       </c>
       <c r="O13" t="n">
         <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>0</v>
+        <v>0.0002603948291765786</v>
       </c>
       <c r="Q13" t="n">
-        <v>0</v>
+        <v>0.00292613172447579</v>
       </c>
       <c r="R13" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.006437048446678642</v>
       </c>
       <c r="S13" t="n">
         <v>0</v>
       </c>
       <c r="T13" t="n">
-        <v>4.763401831051664e-05</v>
+        <v>0.001540301616654677</v>
       </c>
       <c r="U13" t="n">
-        <v>0.001187039736298075</v>
+        <v>0.001813936860874132</v>
       </c>
       <c r="V13" t="n">
-        <v>0</v>
+        <v>0.0003177699610290451</v>
       </c>
       <c r="W13" t="n">
-        <v>3.810721464841331e-05</v>
+        <v>0.0009091751662775456</v>
       </c>
       <c r="X13" t="n">
-        <v>0.0009679232520696981</v>
+        <v>0</v>
       </c>
       <c r="Y13" t="n">
-        <v>2.286432878904799e-05</v>
+        <v>0</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.001326131069764783</v>
+        <v>0</v>
       </c>
       <c r="AA13" t="n">
-        <v>4.763401831051664e-05</v>
+        <v>5.516839601198699e-05</v>
       </c>
       <c r="AB13" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0</v>
       </c>
       <c r="AC13" t="n">
-        <v>1.714824659178599e-05</v>
+        <v>0</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.001150837882382082</v>
+        <v>0</v>
       </c>
       <c r="AE13" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="AF13" t="n">
         <v>0</v>
@@ -1879,13 +1879,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>0.0002250870557289069</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0003391542103708785</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -1894,13 +1894,13 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>0.004089081512408476</v>
       </c>
       <c r="H14" t="n">
-        <v>0.001646231672811455</v>
+        <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1.10336792023974e-05</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
@@ -1909,73 +1909,73 @@
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>7.621442929682662e-05</v>
+        <v>0.002186875217915164</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0006230529595015577</v>
+        <v>0.001350522334373442</v>
       </c>
       <c r="N14" t="n">
-        <v>0.0040660398029857</v>
+        <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>4.001257538083398e-05</v>
+        <v>0</v>
       </c>
       <c r="P14" t="n">
         <v>0</v>
       </c>
       <c r="Q14" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="R14" t="n">
         <v>0</v>
       </c>
       <c r="S14" t="n">
-        <v>0</v>
+        <v>0.005225550470255407</v>
       </c>
       <c r="T14" t="n">
-        <v>1.714824659178599e-05</v>
+        <v>0</v>
       </c>
       <c r="U14" t="n">
-        <v>0.001179418293368392</v>
+        <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>4.572865757809597e-05</v>
+        <v>0</v>
       </c>
       <c r="W14" t="n">
-        <v>0.0001009841188182953</v>
+        <v>0</v>
       </c>
       <c r="X14" t="n">
-        <v>0.0001181323654100813</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.001644326312079034</v>
+        <v>0</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.0009317213981537055</v>
+        <v>0</v>
       </c>
       <c r="AA14" t="n">
-        <v>5.144473977535797e-05</v>
+        <v>0</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.0001067002010155573</v>
+        <v>0</v>
       </c>
       <c r="AC14" t="n">
         <v>0</v>
       </c>
       <c r="AD14" t="n">
-        <v>1.714824659178599e-05</v>
+        <v>0</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.0003486810140329818</v>
+        <v>0</v>
       </c>
       <c r="AF14" t="n">
         <v>0</v>
       </c>
       <c r="AG14" t="n">
-        <v>0</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="AH14" t="n">
-        <v>0.0006630655348823916</v>
+        <v>2.206735840479479e-06</v>
       </c>
     </row>
     <row r="15">
@@ -1985,103 +1985,103 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.006503250521893027</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>0.000105923320343015</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0003315327674411958</v>
+        <v>0.0007855979592106947</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0003620185391599265</v>
+        <v>6.840881105486387e-05</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>0.0002317072632503453</v>
       </c>
       <c r="G15" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.003374099100093124</v>
       </c>
       <c r="H15" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>0.0004303134888934985</v>
       </c>
       <c r="J15" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>3.972124512863063e-05</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>0.0001632984521954815</v>
       </c>
       <c r="L15" t="n">
-        <v>0.001895833928758562</v>
+        <v>0.002873170064304282</v>
       </c>
       <c r="M15" t="n">
-        <v>0.0004058418360056018</v>
+        <v>0.0003994191871267858</v>
       </c>
       <c r="N15" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.0004943088282674034</v>
       </c>
       <c r="O15" t="n">
-        <v>0.008757037926205379</v>
+        <v>0.000271428508378976</v>
       </c>
       <c r="P15" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.0002030196973241121</v>
       </c>
       <c r="Q15" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.0004612077906602112</v>
       </c>
       <c r="R15" t="n">
-        <v>0.006453456800708794</v>
+        <v>0.001533681409133238</v>
       </c>
       <c r="S15" t="n">
-        <v>0</v>
+        <v>0.002140533765265095</v>
       </c>
       <c r="T15" t="n">
-        <v>1.714824659178599e-05</v>
+        <v>2.648083008575376e-05</v>
       </c>
       <c r="U15" t="n">
-        <v>0.001114636028466089</v>
+        <v>0.0004303134888934985</v>
       </c>
       <c r="V15" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0.003826479947391418</v>
       </c>
       <c r="W15" t="n">
-        <v>3.048577171873065e-05</v>
+        <v>0.000809872053455969</v>
       </c>
       <c r="X15" t="n">
-        <v>0.0004325168862594911</v>
+        <v>0.001015098486620561</v>
       </c>
       <c r="Y15" t="n">
         <v>0</v>
       </c>
       <c r="Z15" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0.0002758419800599349</v>
       </c>
       <c r="AA15" t="n">
-        <v>0</v>
+        <v>1.10336792023974e-05</v>
       </c>
       <c r="AB15" t="n">
-        <v>8.764659369135062e-05</v>
+        <v>0.0002559813574956197</v>
       </c>
       <c r="AC15" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.0004391404322554164</v>
       </c>
       <c r="AD15" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0</v>
       </c>
       <c r="AE15" t="n">
-        <v>8.955195442377128e-05</v>
+        <v>0</v>
       </c>
       <c r="AF15" t="n">
-        <v>8.002515076166795e-05</v>
+        <v>0.001121021806963576</v>
       </c>
       <c r="AG15" t="n">
-        <v>0</v>
+        <v>0.0002692217725384965</v>
       </c>
       <c r="AH15" t="n">
-        <v>0</v>
+        <v>0.0009930311282157658</v>
       </c>
     </row>
     <row r="16">
@@ -2091,103 +2091,103 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.006706869778120743</v>
+        <v>0.004265620379646834</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0002267379271580592</v>
+        <v>0.001028338901663437</v>
       </c>
       <c r="D16" t="n">
-        <v>0.001610029818895462</v>
+        <v>0.002921718252794831</v>
       </c>
       <c r="E16" t="n">
-        <v>0.004927262854039841</v>
+        <v>0.0005627176393222673</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>0.001039372580865835</v>
       </c>
       <c r="G16" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>0.007008593029362827</v>
       </c>
       <c r="H16" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>0.0001875725464407558</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0009374374803509674</v>
+        <v>0.0004457606397768549</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0001714824659178599</v>
+        <v>0.001917653445376668</v>
       </c>
       <c r="M16" t="n">
-        <v>0.003336286642468585</v>
+        <v>0.0006333331862176106</v>
       </c>
       <c r="N16" t="n">
-        <v>0.0001276591690721846</v>
+        <v>0.0001412310937906867</v>
       </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>0.0007238093556772693</v>
       </c>
       <c r="P16" t="n">
-        <v>0.003742128478474187</v>
+        <v>0.0002427409424527427</v>
       </c>
       <c r="Q16" t="n">
-        <v>0</v>
+        <v>0.0002295005274098659</v>
       </c>
       <c r="R16" t="n">
-        <v>0.0008021568683491001</v>
+        <v>3.751450928815116e-05</v>
       </c>
       <c r="S16" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>0.005514632865358219</v>
       </c>
       <c r="T16" t="n">
-        <v>0</v>
+        <v>0.0005031357716293214</v>
       </c>
       <c r="U16" t="n">
-        <v>0.0004268008040622291</v>
+        <v>3.751450928815116e-05</v>
       </c>
       <c r="V16" t="n">
-        <v>1.905360732420665e-05</v>
+        <v>0.004413471680958959</v>
       </c>
       <c r="W16" t="n">
-        <v>2.095896805662732e-05</v>
+        <v>0.0003839720362434294</v>
       </c>
       <c r="X16" t="n">
-        <v>1.333752512694466e-05</v>
+        <v>0.0006222995070152132</v>
       </c>
       <c r="Y16" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0.0001677119238764405</v>
       </c>
       <c r="Z16" t="n">
-        <v>9.526803662103327e-06</v>
+        <v>0.0001588849805145225</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.0003715453428220298</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AB16" t="n">
-        <v>2.095896805662732e-05</v>
+        <v>2.648083008575376e-05</v>
       </c>
       <c r="AC16" t="n">
-        <v>0</v>
+        <v>0.000156678244674043</v>
       </c>
       <c r="AD16" t="n">
-        <v>1.905360732420665e-05</v>
+        <v>0</v>
       </c>
       <c r="AE16" t="n">
         <v>0</v>
       </c>
       <c r="AF16" t="n">
-        <v>0</v>
+        <v>9.488964114061763e-05</v>
       </c>
       <c r="AG16" t="n">
-        <v>0</v>
+        <v>5.516839601198699e-05</v>
       </c>
       <c r="AH16" t="n">
-        <v>0.0001505234978612326</v>
+        <v>0.0003663181495195936</v>
       </c>
     </row>
     <row r="17">
@@ -2197,103 +2197,103 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.001510951060809588</v>
+        <v>0.002701044668746883</v>
       </c>
       <c r="C17" t="n">
-        <v>0.005093029237760439</v>
+        <v>3.972124512863063e-05</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>0.0004567943189792523</v>
       </c>
       <c r="E17" t="n">
-        <v>0.002465536787752341</v>
+        <v>1.10336792023974e-05</v>
       </c>
       <c r="F17" t="n">
-        <v>0.001446168795907285</v>
+        <v>0.0004303134888934985</v>
       </c>
       <c r="G17" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.006251682636078366</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0007392799641792183</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>3.530777344767167e-05</v>
       </c>
       <c r="J17" t="n">
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.00289233759181457</v>
+        <v>0.00135714254189488</v>
       </c>
       <c r="L17" t="n">
-        <v>0.001227052311678909</v>
+        <v>0.005861090392313498</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0008764659369135062</v>
+        <v>0.002255284028970028</v>
       </c>
       <c r="N17" t="n">
-        <v>0.0009850714986614842</v>
+        <v>0.0004170730738506216</v>
       </c>
       <c r="O17" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0.0002295005274098659</v>
       </c>
       <c r="P17" t="n">
-        <v>0.004887250278659007</v>
+        <v>1.544715088335636e-05</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.0008021568683491001</v>
+        <v>0.0003729383570410321</v>
       </c>
       <c r="R17" t="n">
-        <v>0.002452199262625397</v>
+        <v>2.427409424527428e-05</v>
       </c>
       <c r="S17" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>0.006031009052030418</v>
       </c>
       <c r="T17" t="n">
-        <v>0.0004401383291891737</v>
+        <v>1.10336792023974e-05</v>
       </c>
       <c r="U17" t="n">
-        <v>0</v>
+        <v>0.001083507297675425</v>
       </c>
       <c r="V17" t="n">
-        <v>0</v>
+        <v>0.0007833912233702153</v>
       </c>
       <c r="W17" t="n">
-        <v>0.0002762773062009965</v>
+        <v>0.0003464575269552783</v>
       </c>
       <c r="X17" t="n">
-        <v>0.0001448074156639706</v>
+        <v>0.0005450637525984314</v>
       </c>
       <c r="Y17" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>1.324041504287688e-05</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.0001829146303123839</v>
+        <v>0.0002559813574956197</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.0002210218449607972</v>
+        <v>1.10336792023974e-05</v>
       </c>
       <c r="AB17" t="n">
-        <v>2.667505025388932e-05</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AC17" t="n">
         <v>0</v>
       </c>
       <c r="AD17" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="AE17" t="n">
         <v>0</v>
       </c>
       <c r="AF17" t="n">
-        <v>0</v>
+        <v>0.0003464575269552783</v>
       </c>
       <c r="AG17" t="n">
-        <v>0</v>
+        <v>9.488964114061763e-05</v>
       </c>
       <c r="AH17" t="n">
-        <v>0.004597635447331066</v>
+        <v>0.001094540976877822</v>
       </c>
     </row>
     <row r="18">
@@ -2303,103 +2303,103 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.004182266807663361</v>
+        <v>0.007754469743444892</v>
       </c>
       <c r="C18" t="n">
-        <v>0.003629712195261368</v>
+        <v>0.0006443668654200081</v>
       </c>
       <c r="D18" t="n">
-        <v>8.383587222650928e-05</v>
+        <v>0.003268175779750109</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>0.0002096399048455506</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>0.001597676748507143</v>
       </c>
       <c r="G18" t="n">
-        <v>0.002092086084197891</v>
+        <v>0.01652624470935082</v>
       </c>
       <c r="H18" t="n">
-        <v>0.001009841188182953</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>0.0001390243579502072</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>0.001436585032152141</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>0.002957026026242503</v>
       </c>
       <c r="L18" t="n">
-        <v>0.0001943467947069079</v>
+        <v>0.004618698114123551</v>
       </c>
       <c r="M18" t="n">
-        <v>0.0009355321196185468</v>
+        <v>0.0004766549415435676</v>
       </c>
       <c r="N18" t="n">
-        <v>4.763401831051664e-05</v>
+        <v>0.000699535261431995</v>
       </c>
       <c r="O18" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>0.0006311264503771312</v>
       </c>
       <c r="P18" t="n">
-        <v>0</v>
+        <v>0.0004766549415435676</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.001909171453885507</v>
+        <v>0.001246805749870906</v>
       </c>
       <c r="R18" t="n">
-        <v>0.008429315880229025</v>
+        <v>0.005627176393222673</v>
       </c>
       <c r="S18" t="n">
-        <v>0.0003048577171873065</v>
+        <v>0.005124040621593351</v>
       </c>
       <c r="T18" t="n">
-        <v>8.383587222650928e-05</v>
+        <v>0.0001213704712263714</v>
       </c>
       <c r="U18" t="n">
-        <v>0</v>
+        <v>0.0006200927711747338</v>
       </c>
       <c r="V18" t="n">
-        <v>0</v>
+        <v>0.001363762749416318</v>
       </c>
       <c r="W18" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0.003325550911602576</v>
       </c>
       <c r="X18" t="n">
-        <v>0.0001810092695799632</v>
+        <v>0.001030545637503917</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.0001086055617479779</v>
+        <v>2.20673584047948e-05</v>
       </c>
       <c r="Z18" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>0.000487688620745965</v>
       </c>
       <c r="AA18" t="n">
-        <v>0</v>
+        <v>2.20673584047948e-05</v>
       </c>
       <c r="AB18" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>0.001348315598532962</v>
       </c>
       <c r="AC18" t="n">
-        <v>3.810721464841331e-05</v>
+        <v>0.0004104528663291832</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.001878685682166776</v>
+        <v>8.826943361917918e-05</v>
       </c>
       <c r="AE18" t="n">
         <v>0</v>
       </c>
       <c r="AF18" t="n">
-        <v>0</v>
+        <v>0.005911845316644525</v>
       </c>
       <c r="AG18" t="n">
-        <v>0</v>
+        <v>0.0001699186597169199</v>
       </c>
       <c r="AH18" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.001599883484347623</v>
       </c>
     </row>
     <row r="19">
@@ -2409,103 +2409,103 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.009460116036468605</v>
+        <v>0.001041579316706314</v>
       </c>
       <c r="C19" t="n">
-        <v>0.002036830622957691</v>
+        <v>0.002482577820539414</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0008497908866596168</v>
+        <v>0.00903437653092299</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0002172111234959559</v>
+        <v>0.007833912233702153</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>0.002606155027606266</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0003258166852439338</v>
+        <v>0.002535539480710922</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0001371859727342879</v>
+        <v>0</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>1.10336792023974e-05</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>0.0008849010720322713</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>0.002453890254613181</v>
       </c>
       <c r="M19" t="n">
-        <v>0.005083502434098336</v>
+        <v>0.0004038326588077448</v>
       </c>
       <c r="N19" t="n">
-        <v>0.0001333752512694466</v>
+        <v>0.0008407663552226817</v>
       </c>
       <c r="O19" t="n">
-        <v>0</v>
+        <v>0.008968174455708605</v>
       </c>
       <c r="P19" t="n">
-        <v>0.0001162270046776606</v>
+        <v>0.00572647950604425</v>
       </c>
       <c r="Q19" t="n">
-        <v>0</v>
+        <v>0.005377815243248492</v>
       </c>
       <c r="R19" t="n">
-        <v>0.001768174759686378</v>
+        <v>0.01685284161374179</v>
       </c>
       <c r="S19" t="n">
-        <v>0.001025084074042318</v>
+        <v>0.00292392498863531</v>
       </c>
       <c r="T19" t="n">
-        <v>0.0008135890327436242</v>
+        <v>0.008173749553135993</v>
       </c>
       <c r="U19" t="n">
-        <v>0.0001067002010155573</v>
+        <v>0.008019278044302429</v>
       </c>
       <c r="V19" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.005704412147639454</v>
       </c>
       <c r="W19" t="n">
-        <v>0</v>
+        <v>0.01398187828527798</v>
       </c>
       <c r="X19" t="n">
-        <v>0</v>
+        <v>0.0003905922437648679</v>
       </c>
       <c r="Y19" t="n">
-        <v>0</v>
+        <v>0.0009952378640562453</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.001451884878104547</v>
+        <v>0.003248315157185794</v>
       </c>
       <c r="AA19" t="n">
-        <v>0</v>
+        <v>2.868756592623324e-05</v>
       </c>
       <c r="AB19" t="n">
-        <v>0</v>
+        <v>1.765388672383584e-05</v>
       </c>
       <c r="AC19" t="n">
-        <v>0</v>
+        <v>0.0001213704712263714</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.000501109872626635</v>
+        <v>0</v>
       </c>
       <c r="AE19" t="n">
-        <v>2.476968952146865e-05</v>
+        <v>0</v>
       </c>
       <c r="AF19" t="n">
-        <v>0</v>
+        <v>0.0005252031300341161</v>
       </c>
       <c r="AG19" t="n">
-        <v>0</v>
+        <v>0.0003420440552743193</v>
       </c>
       <c r="AH19" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.001041579316706314</v>
       </c>
     </row>
     <row r="20">
@@ -2515,103 +2515,103 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.01251631465127135</v>
+        <v>0.002676770574501609</v>
       </c>
       <c r="C20" t="n">
-        <v>0.006080006097154343</v>
+        <v>2.427409424527428e-05</v>
       </c>
       <c r="D20" t="n">
-        <v>3.429649318357198e-05</v>
+        <v>0.001032752373344396</v>
       </c>
       <c r="E20" t="n">
-        <v>0.002456009984090238</v>
+        <v>2.20673584047948e-05</v>
       </c>
       <c r="F20" t="n">
-        <v>3.810721464841331e-05</v>
+        <v>0.0001721253955573994</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>0.003239488213823876</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>1.765388672383584e-05</v>
       </c>
       <c r="J20" t="n">
         <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>0.0001279906787478098</v>
       </c>
       <c r="L20" t="n">
-        <v>0</v>
+        <v>0.002319279368343933</v>
       </c>
       <c r="M20" t="n">
-        <v>0</v>
+        <v>0.0008297326760202844</v>
       </c>
       <c r="N20" t="n">
-        <v>0.001991101965379596</v>
+        <v>0.001304180881723372</v>
       </c>
       <c r="O20" t="n">
-        <v>5.716082197261997e-05</v>
+        <v>0.000483275149065006</v>
       </c>
       <c r="P20" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.000105923320343015</v>
       </c>
       <c r="Q20" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.001160743052092206</v>
       </c>
       <c r="R20" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>0.0001500580371526046</v>
       </c>
       <c r="S20" t="n">
-        <v>0.008370249697523984</v>
+        <v>0.005141694508317187</v>
       </c>
       <c r="T20" t="n">
-        <v>0.01681099774214753</v>
+        <v>0.000262601565017058</v>
       </c>
       <c r="U20" t="n">
-        <v>0.000518258119218421</v>
+        <v>0.0001257839429073303</v>
       </c>
       <c r="V20" t="n">
-        <v>0</v>
+        <v>0.003023228101456887</v>
       </c>
       <c r="W20" t="n">
-        <v>0.0002343593700877418</v>
+        <v>0.0008473865627441202</v>
       </c>
       <c r="X20" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>0.00123135859898755</v>
       </c>
       <c r="Y20" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.0001143216439452399</v>
+        <v>0.0008606269777869971</v>
       </c>
       <c r="AA20" t="n">
-        <v>0</v>
+        <v>1.544715088335636e-05</v>
       </c>
       <c r="AB20" t="n">
-        <v>0</v>
+        <v>8.826943361917918e-06</v>
       </c>
       <c r="AC20" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AD20" t="n">
         <v>0</v>
       </c>
       <c r="AE20" t="n">
-        <v>5.906618270504063e-05</v>
+        <v>0</v>
       </c>
       <c r="AF20" t="n">
-        <v>0</v>
+        <v>0.0007436699782415846</v>
       </c>
       <c r="AG20" t="n">
-        <v>0</v>
+        <v>0.0002934958667837708</v>
       </c>
       <c r="AH20" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.001504993843207005</v>
       </c>
     </row>
     <row r="21">
@@ -2621,88 +2621,88 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.01464269722865282</v>
+        <v>0.001944134275462421</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0001295645298046053</v>
+        <v>0.001368176221097277</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0005677974982613584</v>
+        <v>0.0008672471853084355</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0002229272056932179</v>
+        <v>0.001048199524227753</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0004972991511617937</v>
+        <v>0.001421137881268785</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0001371859727342879</v>
+        <v>0.007015213236884266</v>
       </c>
       <c r="H21" t="n">
-        <v>0.003593510341345375</v>
+        <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>1.10336792023974e-05</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>0.0006289197145366517</v>
       </c>
       <c r="L21" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>0.002231009934724754</v>
       </c>
       <c r="M21" t="n">
-        <v>2.476968952146865e-05</v>
+        <v>0.0005715445826841852</v>
       </c>
       <c r="N21" t="n">
-        <v>0</v>
+        <v>0.0004943088282674034</v>
       </c>
       <c r="O21" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.001169569995454124</v>
       </c>
       <c r="P21" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>3.751450928815116e-05</v>
       </c>
       <c r="Q21" t="n">
-        <v>1.905360732420665e-05</v>
+        <v>0.0003398373194338398</v>
       </c>
       <c r="R21" t="n">
-        <v>2.476968952146865e-05</v>
+        <v>7.502901857630231e-05</v>
       </c>
       <c r="S21" t="n">
-        <v>0</v>
+        <v>0.007758883215125851</v>
       </c>
       <c r="T21" t="n">
-        <v>2.476968952146865e-05</v>
+        <v>0.009727291584833545</v>
       </c>
       <c r="U21" t="n">
-        <v>0.0002629397810740519</v>
+        <v>4.413471680958959e-05</v>
       </c>
       <c r="V21" t="n">
-        <v>5.144473977535797e-05</v>
+        <v>0.001162949787932686</v>
       </c>
       <c r="W21" t="n">
-        <v>9.526803662103327e-06</v>
+        <v>0.003616840042545867</v>
       </c>
       <c r="X21" t="n">
-        <v>0.0007926300646869969</v>
+        <v>0.0006598140163033644</v>
       </c>
       <c r="Y21" t="n">
-        <v>0</v>
+        <v>5.737513185246647e-05</v>
       </c>
       <c r="Z21" t="n">
-        <v>0.001074623453085255</v>
+        <v>0.0005450637525984314</v>
       </c>
       <c r="AA21" t="n">
-        <v>0</v>
+        <v>1.10336792023974e-05</v>
       </c>
       <c r="AB21" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>3.751450928815116e-05</v>
       </c>
       <c r="AC21" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AD21" t="n">
         <v>0</v>
@@ -2711,13 +2711,13 @@
         <v>0</v>
       </c>
       <c r="AF21" t="n">
-        <v>0.0004039364752731811</v>
+        <v>0.0001875725464407558</v>
       </c>
       <c r="AG21" t="n">
-        <v>0</v>
+        <v>0.0001191637353858919</v>
       </c>
       <c r="AH21" t="n">
-        <v>0.000603999352177351</v>
+        <v>0.0006024388844508979</v>
       </c>
     </row>
     <row r="22">
@@ -2727,88 +2727,88 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.005662732096754218</v>
+        <v>0.002985713592168736</v>
       </c>
       <c r="C22" t="n">
-        <v>0.001255632722665219</v>
+        <v>0.000326596904390963</v>
       </c>
       <c r="D22" t="n">
-        <v>0.00214734154543809</v>
+        <v>0.002897444158549557</v>
       </c>
       <c r="E22" t="n">
-        <v>0.002356931226004363</v>
+        <v>4.634145265006907e-05</v>
       </c>
       <c r="F22" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0.001288733730840016</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0008917088227728715</v>
+        <v>0.009630195207852448</v>
       </c>
       <c r="H22" t="n">
-        <v>0.002097802166395153</v>
+        <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>8.826943361917918e-06</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
       </c>
       <c r="K22" t="n">
-        <v>0.00183295702458868</v>
+        <v>0.000110336792023974</v>
       </c>
       <c r="L22" t="n">
-        <v>2.095896805662732e-05</v>
+        <v>0.005962600240975554</v>
       </c>
       <c r="M22" t="n">
-        <v>0.0004763401831051664</v>
+        <v>0.001540301616654677</v>
       </c>
       <c r="N22" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0.003665388231036416</v>
       </c>
       <c r="O22" t="n">
-        <v>0</v>
+        <v>0.001134262222006453</v>
       </c>
       <c r="P22" t="n">
-        <v>0.0002686558632713138</v>
+        <v>0.000271428508378976</v>
       </c>
       <c r="Q22" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0.00122915186314707</v>
       </c>
       <c r="R22" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>0.0006554005446224054</v>
       </c>
       <c r="S22" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0.01140661755943843</v>
       </c>
       <c r="T22" t="n">
-        <v>0.005695123229205369</v>
+        <v>0.001118815071123096</v>
       </c>
       <c r="U22" t="n">
-        <v>0.001047948402831366</v>
+        <v>0.0002317072632503453</v>
       </c>
       <c r="V22" t="n">
-        <v>0.0008459801651947755</v>
+        <v>0.002520092329827566</v>
       </c>
       <c r="W22" t="n">
-        <v>0.0005201634799508417</v>
+        <v>0.004415678416799439</v>
       </c>
       <c r="X22" t="n">
-        <v>4.763401831051664e-05</v>
+        <v>0.002014749822357765</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.004161307839606733</v>
+        <v>6.620207521438439e-05</v>
       </c>
       <c r="Z22" t="n">
-        <v>0</v>
+        <v>0.001112194863601658</v>
       </c>
       <c r="AA22" t="n">
-        <v>0</v>
+        <v>1.986062256431532e-05</v>
       </c>
       <c r="AB22" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AC22" t="n">
-        <v>0</v>
+        <v>6.620207521438439e-06</v>
       </c>
       <c r="AD22" t="n">
         <v>0</v>
@@ -2817,13 +2817,13 @@
         <v>0</v>
       </c>
       <c r="AF22" t="n">
-        <v>0</v>
+        <v>0.001319628032606729</v>
       </c>
       <c r="AG22" t="n">
-        <v>0</v>
+        <v>0.0004082461304887037</v>
       </c>
       <c r="AH22" t="n">
-        <v>0.0004020311145407604</v>
+        <v>0.001710220276371597</v>
       </c>
     </row>
     <row r="23">
@@ -2833,103 +2833,103 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.01460077929253956</v>
+        <v>0.004556909510590125</v>
       </c>
       <c r="C23" t="n">
-        <v>0.001343279316356569</v>
+        <v>8.826943361917918e-06</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>0.001134262222006453</v>
       </c>
       <c r="E23" t="n">
-        <v>0.007055550792153724</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0001600503015233359</v>
+        <v>0.0001125435278644535</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0003563024569626644</v>
+        <v>0.008906385852175179</v>
       </c>
       <c r="H23" t="n">
-        <v>0.005815160955347871</v>
+        <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>0.003738210513772238</v>
       </c>
       <c r="J23" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>4.192798096911011e-05</v>
       </c>
       <c r="L23" t="n">
-        <v>0.0006344851238960816</v>
+        <v>0.006412774352433368</v>
       </c>
       <c r="M23" t="n">
-        <v>0.003536349519372755</v>
+        <v>0.002169221331191329</v>
       </c>
       <c r="N23" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0.0004898953565864445</v>
       </c>
       <c r="O23" t="n">
-        <v>1.714824659178599e-05</v>
+        <v>0.002548779895753799</v>
       </c>
       <c r="P23" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>5.516839601198699e-05</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.005287376032467347</v>
+        <v>0.0003729383570410321</v>
       </c>
       <c r="R23" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.001648431672838171</v>
       </c>
       <c r="S23" t="n">
-        <v>6.478226490230263e-05</v>
+        <v>0.009539719038392791</v>
       </c>
       <c r="T23" t="n">
-        <v>0.008777996894262006</v>
+        <v>0.000156678244674043</v>
       </c>
       <c r="U23" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0.0004678279981816497</v>
       </c>
       <c r="V23" t="n">
-        <v>0.008438842683891128</v>
+        <v>0.0170558613110659</v>
       </c>
       <c r="W23" t="n">
-        <v>0.002415997408709404</v>
+        <v>0.0003641114136791142</v>
       </c>
       <c r="X23" t="n">
-        <v>0.003852639400954586</v>
+        <v>0.001279906787478098</v>
       </c>
       <c r="Y23" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="Z23" t="n">
-        <v>0</v>
+        <v>0.0002228803198884274</v>
       </c>
       <c r="AA23" t="n">
-        <v>0</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="AB23" t="n">
-        <v>0</v>
+        <v>0.00228838506657722</v>
       </c>
       <c r="AC23" t="n">
-        <v>0</v>
+        <v>3.751450928815116e-05</v>
       </c>
       <c r="AD23" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AE23" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0</v>
       </c>
       <c r="AF23" t="n">
-        <v>0</v>
+        <v>0.000708362204793913</v>
       </c>
       <c r="AG23" t="n">
-        <v>0</v>
+        <v>0.001705806804690638</v>
       </c>
       <c r="AH23" t="n">
-        <v>0</v>
+        <v>0.002963646233763941</v>
       </c>
     </row>
     <row r="24">
@@ -2939,103 +2939,103 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.006078100736421923</v>
+        <v>0.0004612077906602112</v>
       </c>
       <c r="C24" t="n">
-        <v>0.001771985481151219</v>
+        <v>0.000754703657443982</v>
       </c>
       <c r="D24" t="n">
-        <v>0.001120352110663351</v>
+        <v>0.001321834768447208</v>
       </c>
       <c r="E24" t="n">
-        <v>0.0002362647308201625</v>
+        <v>0.0002979093384647297</v>
       </c>
       <c r="F24" t="n">
-        <v>0.006786894928882411</v>
+        <v>0.00131521456092577</v>
       </c>
       <c r="G24" t="n">
-        <v>0.001280402412186687</v>
+        <v>0.0005649243751627467</v>
       </c>
       <c r="H24" t="n">
-        <v>0.004685282041022416</v>
+        <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>1.524288585936533e-05</v>
+        <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>0.0003829775072165538</v>
+        <v>0.0001346108862692482</v>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>0.001074680354313507</v>
       </c>
       <c r="L24" t="n">
-        <v>0.0006097154343746129</v>
+        <v>0.0004854818849054855</v>
       </c>
       <c r="M24" t="n">
-        <v>0.002322634732820791</v>
+        <v>0.0001390243579502072</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0001505234978612326</v>
+        <v>0.0001235772070668508</v>
       </c>
       <c r="O24" t="n">
-        <v>0</v>
+        <v>0.000856213506106038</v>
       </c>
       <c r="P24" t="n">
-        <v>0</v>
+        <v>0.001180603674656522</v>
       </c>
       <c r="Q24" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.001924273652898106</v>
       </c>
       <c r="R24" t="n">
-        <v>0.004559528232682653</v>
+        <v>0.001295353938361454</v>
       </c>
       <c r="S24" t="n">
-        <v>0.0002476968952146865</v>
+        <v>0.0004567943189792523</v>
       </c>
       <c r="T24" t="n">
-        <v>0.005636057046500329</v>
+        <v>0.000483275149065006</v>
       </c>
       <c r="U24" t="n">
-        <v>0</v>
+        <v>0.002837862290856611</v>
       </c>
       <c r="V24" t="n">
-        <v>1.333752512694466e-05</v>
+        <v>0.001204877768901796</v>
       </c>
       <c r="W24" t="n">
-        <v>0.001423304467118237</v>
+        <v>0.001981648784750573</v>
       </c>
       <c r="X24" t="n">
-        <v>0.006849771833052292</v>
+        <v>8.826943361917918e-05</v>
       </c>
       <c r="Y24" t="n">
-        <v>0.0002572236988767898</v>
+        <v>0.0004567943189792523</v>
       </c>
       <c r="Z24" t="n">
-        <v>0.001834862385321101</v>
+        <v>0.0003045295459861682</v>
       </c>
       <c r="AA24" t="n">
-        <v>0</v>
+        <v>5.075492433102803e-05</v>
       </c>
       <c r="AB24" t="n">
-        <v>0</v>
+        <v>0.0005649243751627467</v>
       </c>
       <c r="AC24" t="n">
-        <v>0</v>
+        <v>5.958186769294595e-05</v>
       </c>
       <c r="AD24" t="n">
-        <v>1.905360732420665e-05</v>
+        <v>0.0004810684132245266</v>
       </c>
       <c r="AE24" t="n">
         <v>0</v>
       </c>
       <c r="AF24" t="n">
-        <v>0</v>
+        <v>0.000156678244674043</v>
       </c>
       <c r="AG24" t="n">
-        <v>0</v>
+        <v>4.413471680958959e-05</v>
       </c>
       <c r="AH24" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.0003574912061576757</v>
       </c>
     </row>
     <row r="25">
@@ -3045,85 +3045,85 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.003324854478074061</v>
+        <v>0.0001897792822812353</v>
       </c>
       <c r="C25" t="n">
-        <v>0.003513485190583707</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0002286432878904799</v>
+        <v>0.0001522647729930841</v>
       </c>
       <c r="E25" t="n">
-        <v>0.0004439490506540151</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="F25" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>8.826943361917918e-06</v>
       </c>
       <c r="G25" t="n">
-        <v>0.002194975563748607</v>
+        <v>0.0005031357716293214</v>
       </c>
       <c r="H25" t="n">
-        <v>0.01333371440547982</v>
+        <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.0001368176221097277</v>
       </c>
       <c r="J25" t="n">
-        <v>0.0001409966941991293</v>
+        <v>0</v>
       </c>
       <c r="K25" t="n">
-        <v>4.001257538083398e-05</v>
+        <v>1.765388672383584e-05</v>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>0.0005715445826841852</v>
       </c>
       <c r="M25" t="n">
-        <v>0</v>
+        <v>6.399533937390491e-05</v>
       </c>
       <c r="N25" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0.0002648083008575376</v>
       </c>
       <c r="O25" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>4.634145265006907e-05</v>
       </c>
       <c r="P25" t="n">
-        <v>0.0002419808130174245</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="Q25" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0.0001169569995454124</v>
       </c>
       <c r="R25" t="n">
-        <v>0</v>
+        <v>3.31010376071922e-05</v>
       </c>
       <c r="S25" t="n">
-        <v>0.006388674535806492</v>
+        <v>0.0003177699610290451</v>
       </c>
       <c r="T25" t="n">
-        <v>0.004283250926481656</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="U25" t="n">
-        <v>0</v>
+        <v>4.413471680958959e-05</v>
       </c>
       <c r="V25" t="n">
-        <v>0.0006497280097554469</v>
+        <v>0.0001743321313978789</v>
       </c>
       <c r="W25" t="n">
-        <v>4.763401831051664e-05</v>
+        <v>8.385596193822023e-05</v>
       </c>
       <c r="X25" t="n">
-        <v>0.005605571274781598</v>
+        <v>5.296166017150751e-05</v>
       </c>
       <c r="Y25" t="n">
-        <v>0.003595415702077796</v>
+        <v>0.000271428508378976</v>
       </c>
       <c r="Z25" t="n">
-        <v>5.906618270504063e-05</v>
+        <v>0.0001941927539621942</v>
       </c>
       <c r="AA25" t="n">
         <v>0</v>
       </c>
       <c r="AB25" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AC25" t="n">
         <v>0</v>
@@ -3132,16 +3132,16 @@
         <v>0</v>
       </c>
       <c r="AE25" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0</v>
       </c>
       <c r="AF25" t="n">
-        <v>0</v>
+        <v>4.413471680958959e-05</v>
       </c>
       <c r="AG25" t="n">
-        <v>0</v>
+        <v>8.826943361917918e-05</v>
       </c>
       <c r="AH25" t="n">
-        <v>0</v>
+        <v>0.0002096399048455506</v>
       </c>
     </row>
     <row r="26">
@@ -3151,85 +3151,85 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.001914887536082769</v>
+        <v>0.0007238093556772693</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0002038735983690112</v>
+        <v>0.000262601565017058</v>
       </c>
       <c r="D26" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.0001588849805145225</v>
       </c>
       <c r="E26" t="n">
-        <v>0.001625272704754828</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0.0009012356264349748</v>
+        <v>9.047616945965866e-05</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0001257538083397639</v>
+        <v>0.0007348430348796666</v>
       </c>
       <c r="H26" t="n">
-        <v>0.000586851105585565</v>
+        <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="J26" t="n">
-        <v>3.810721464841331e-05</v>
+        <v>0</v>
       </c>
       <c r="K26" t="n">
         <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>0.0001143216439452399</v>
+        <v>0.004453192926087589</v>
       </c>
       <c r="M26" t="n">
-        <v>0.001893928568026142</v>
+        <v>0.00317990634613093</v>
       </c>
       <c r="N26" t="n">
-        <v>0</v>
+        <v>8.826943361917918e-05</v>
       </c>
       <c r="O26" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>1.324041504287688e-05</v>
       </c>
       <c r="P26" t="n">
-        <v>1.524288585936533e-05</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.0002076843198338525</v>
+        <v>3.530777344767167e-05</v>
       </c>
       <c r="R26" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>1.324041504287688e-05</v>
       </c>
       <c r="S26" t="n">
-        <v>0</v>
+        <v>0.0003045295459861682</v>
       </c>
       <c r="T26" t="n">
-        <v>0.002469347509217183</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="U26" t="n">
-        <v>0</v>
+        <v>9.488964114061763e-05</v>
       </c>
       <c r="V26" t="n">
-        <v>0.000621147598769137</v>
+        <v>0.0004700347340221291</v>
       </c>
       <c r="W26" t="n">
-        <v>0.002034925262225271</v>
+        <v>5.296166017150751e-05</v>
       </c>
       <c r="X26" t="n">
-        <v>3.239113245115131e-05</v>
+        <v>0.0002449476782932222</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.0002953309135252031</v>
+        <v>0</v>
       </c>
       <c r="Z26" t="n">
-        <v>4.763401831051664e-05</v>
+        <v>1.765388672383584e-05</v>
       </c>
       <c r="AA26" t="n">
         <v>0</v>
       </c>
       <c r="AB26" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="AC26" t="n">
         <v>0</v>
@@ -3241,13 +3241,13 @@
         <v>0</v>
       </c>
       <c r="AF26" t="n">
-        <v>0</v>
+        <v>2.868756592623324e-05</v>
       </c>
       <c r="AG26" t="n">
-        <v>0</v>
+        <v>1.544715088335636e-05</v>
       </c>
       <c r="AH26" t="n">
-        <v>2.095896805662732e-05</v>
+        <v>0.0006554005446224054</v>
       </c>
     </row>
     <row r="27">
@@ -3257,103 +3257,103 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.000684024502939019</v>
+        <v>0.0007745642800082973</v>
       </c>
       <c r="C27" t="n">
-        <v>9.717339735345395e-05</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0006344851238960816</v>
+        <v>8.385596193822023e-05</v>
       </c>
       <c r="E27" t="n">
-        <v>0.0004039364752731811</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
+        <v>1.544715088335636e-05</v>
       </c>
       <c r="G27" t="n">
-        <v>0.001234673754608591</v>
+        <v>0.0006046456202913774</v>
       </c>
       <c r="H27" t="n">
-        <v>0.0009488696447454915</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>0.0001181323654100813</v>
+        <v>1.10336792023974e-05</v>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="L27" t="n">
-        <v>0.0003963150323434984</v>
+        <v>0.0003619046778386346</v>
       </c>
       <c r="M27" t="n">
-        <v>0.0016043137366982</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="N27" t="n">
-        <v>0.001143216439452399</v>
+        <v>7.944249025726126e-05</v>
       </c>
       <c r="O27" t="n">
-        <v>0</v>
+        <v>0.000750290185763023</v>
       </c>
       <c r="P27" t="n">
-        <v>0.002770394504939648</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="Q27" t="n">
-        <v>0</v>
+        <v>2.427409424527428e-05</v>
       </c>
       <c r="R27" t="n">
-        <v>0</v>
+        <v>0.0004457606397768549</v>
       </c>
       <c r="S27" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.001429964824630703</v>
       </c>
       <c r="T27" t="n">
-        <v>0</v>
+        <v>5.737513185246647e-05</v>
       </c>
       <c r="U27" t="n">
-        <v>0.002840892852039212</v>
+        <v>3.972124512863063e-05</v>
       </c>
       <c r="V27" t="n">
-        <v>2.858041098630998e-05</v>
+        <v>1.765388672383584e-05</v>
       </c>
       <c r="W27" t="n">
-        <v>9.526803662103327e-06</v>
+        <v>2.868756592623324e-05</v>
       </c>
       <c r="X27" t="n">
-        <v>0.005662732096754218</v>
+        <v>1.986062256431532e-05</v>
       </c>
       <c r="Y27" t="n">
-        <v>0.0003448702925681404</v>
+        <v>0</v>
       </c>
       <c r="Z27" t="n">
-        <v>0.0003715453428220298</v>
+        <v>3.972124512863063e-05</v>
       </c>
       <c r="AA27" t="n">
-        <v>0.006666857202739909</v>
+        <v>0</v>
       </c>
       <c r="AB27" t="n">
         <v>0</v>
       </c>
       <c r="AC27" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AD27" t="n">
-        <v>7.621442929682662e-05</v>
+        <v>0</v>
       </c>
       <c r="AE27" t="n">
         <v>0</v>
       </c>
       <c r="AF27" t="n">
-        <v>0</v>
+        <v>3.31010376071922e-05</v>
       </c>
       <c r="AG27" t="n">
-        <v>0</v>
+        <v>8.606269777869971e-05</v>
       </c>
       <c r="AH27" t="n">
-        <v>1.333752512694466e-05</v>
+        <v>0.0001125435278644535</v>
       </c>
     </row>
     <row r="28">
@@ -3363,85 +3363,85 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.0004229900825973877</v>
+        <v>0.001899999558652832</v>
       </c>
       <c r="C28" t="n">
-        <v>0.0005658921375289377</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>0.0001588849805145225</v>
       </c>
       <c r="E28" t="n">
-        <v>0.001009841188182953</v>
+        <v>6.620207521438439e-06</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>0.0001875725464407558</v>
       </c>
       <c r="G28" t="n">
-        <v>0.001093677060409462</v>
+        <v>0.001763181936543104</v>
       </c>
       <c r="H28" t="n">
-        <v>0.005357874379566911</v>
+        <v>0</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="K28" t="n">
-        <v>0.001282307772919108</v>
+        <v>3.089430176671271e-05</v>
       </c>
       <c r="L28" t="n">
-        <v>0.001217525508016805</v>
+        <v>0.003991985135427378</v>
       </c>
       <c r="M28" t="n">
-        <v>0.001530004668133794</v>
+        <v>0.0002890823951028118</v>
       </c>
       <c r="N28" t="n">
-        <v>0.0001924414339744872</v>
+        <v>0.0003332171119124014</v>
       </c>
       <c r="O28" t="n">
-        <v>0</v>
+        <v>0.0001434378296311662</v>
       </c>
       <c r="P28" t="n">
-        <v>0</v>
+        <v>4.192798096911011e-05</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.00426419731915745</v>
+        <v>0.0005803715260461032</v>
       </c>
       <c r="R28" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>6.399533937390491e-05</v>
       </c>
       <c r="S28" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0.002063298010848313</v>
       </c>
       <c r="T28" t="n">
-        <v>0.0002476968952146865</v>
+        <v>1.765388672383584e-05</v>
       </c>
       <c r="U28" t="n">
-        <v>0</v>
+        <v>5.296166017150751e-05</v>
       </c>
       <c r="V28" t="n">
-        <v>0.007918679203940286</v>
+        <v>0.0002008129614836326</v>
       </c>
       <c r="W28" t="n">
-        <v>0.0001200377261425019</v>
+        <v>0.0003067362818266477</v>
       </c>
       <c r="X28" t="n">
-        <v>9.526803662103327e-06</v>
+        <v>0.001922066917057627</v>
       </c>
       <c r="Y28" t="n">
-        <v>0.0005087313155563177</v>
+        <v>0</v>
       </c>
       <c r="Z28" t="n">
-        <v>0</v>
+        <v>0.0001257839429073303</v>
       </c>
       <c r="AA28" t="n">
-        <v>0.000598283269980089</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="AB28" t="n">
-        <v>0.0001371859727342879</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AC28" t="n">
         <v>0</v>
@@ -3450,16 +3450,16 @@
         <v>0</v>
       </c>
       <c r="AE28" t="n">
-        <v>0.0003410595711032991</v>
+        <v>0</v>
       </c>
       <c r="AF28" t="n">
-        <v>0</v>
+        <v>0.0002824621875813734</v>
       </c>
       <c r="AG28" t="n">
-        <v>0</v>
+        <v>0.0004435539039363754</v>
       </c>
       <c r="AH28" t="n">
-        <v>0.0003029523564548858</v>
+        <v>0.0003883855079243884</v>
       </c>
     </row>
     <row r="29">
@@ -3469,88 +3469,88 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.00392313774805415</v>
+        <v>0.0004236932813720601</v>
       </c>
       <c r="C29" t="n">
-        <v>0.0006306744024312403</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0002229272056932179</v>
+        <v>0.000271428508378976</v>
       </c>
       <c r="E29" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="F29" t="n">
-        <v>0.0003010469957224652</v>
+        <v>0.0001169569995454124</v>
       </c>
       <c r="G29" t="n">
-        <v>6.478226490230263e-05</v>
+        <v>0.0008120787892964484</v>
       </c>
       <c r="H29" t="n">
-        <v>0.006588737412710662</v>
+        <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>0</v>
       </c>
       <c r="K29" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>2.648083008575376e-05</v>
       </c>
       <c r="L29" t="n">
-        <v>0.002467442148484762</v>
+        <v>0.0004523808472982933</v>
       </c>
       <c r="M29" t="n">
-        <v>0.004388045766764792</v>
+        <v>0.0002780487159004144</v>
       </c>
       <c r="N29" t="n">
-        <v>0.000535406365810207</v>
+        <v>0.0003861787720839089</v>
       </c>
       <c r="O29" t="n">
-        <v>4.95393790429373e-05</v>
+        <v>3.751450928815116e-05</v>
       </c>
       <c r="P29" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.0002457915344822659</v>
+        <v>2.648083008575376e-05</v>
       </c>
       <c r="R29" t="n">
-        <v>0.003241018605847552</v>
+        <v>2.427409424527428e-05</v>
       </c>
       <c r="S29" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0.001253425957392344</v>
       </c>
       <c r="T29" t="n">
-        <v>0.001951089389998762</v>
+        <v>8.826943361917918e-06</v>
       </c>
       <c r="U29" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.0002824621875813734</v>
       </c>
       <c r="V29" t="n">
-        <v>0</v>
+        <v>0.0002361207349313043</v>
       </c>
       <c r="W29" t="n">
-        <v>0.001743405070164909</v>
+        <v>6.620207521438439e-06</v>
       </c>
       <c r="X29" t="n">
-        <v>0.0002229272056932179</v>
+        <v>0.0001721253955573994</v>
       </c>
       <c r="Y29" t="n">
-        <v>0.0008993302657025541</v>
+        <v>0</v>
       </c>
       <c r="Z29" t="n">
-        <v>0</v>
+        <v>1.10336792023974e-05</v>
       </c>
       <c r="AA29" t="n">
         <v>0</v>
       </c>
       <c r="AB29" t="n">
-        <v>0.0001581449407909152</v>
+        <v>2.427409424527428e-05</v>
       </c>
       <c r="AC29" t="n">
-        <v>8.002515076166795e-05</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="AD29" t="n">
         <v>0</v>
@@ -3559,13 +3559,13 @@
         <v>0</v>
       </c>
       <c r="AF29" t="n">
-        <v>7.240370783198529e-05</v>
+        <v>0.0003486642627957578</v>
       </c>
       <c r="AG29" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AH29" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>2.20673584047948e-05</v>
       </c>
     </row>
     <row r="30">
@@ -3575,103 +3575,103 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.0003143845208494098</v>
+        <v>0.0003883855079243884</v>
       </c>
       <c r="C30" t="n">
-        <v>0.001478559928358437</v>
+        <v>0.0009974445998967249</v>
       </c>
       <c r="D30" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="E30" t="n">
-        <v>4.572865757809597e-05</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>0.001118446749930931</v>
+        <v>0.0006598140163033644</v>
       </c>
       <c r="H30" t="n">
-        <v>0.006884068326235865</v>
+        <v>0</v>
       </c>
       <c r="I30" t="n">
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="L30" t="n">
-        <v>0.0007335638819819562</v>
+        <v>9.488964114061763e-05</v>
       </c>
       <c r="M30" t="n">
-        <v>0.002964741299646556</v>
+        <v>0</v>
       </c>
       <c r="N30" t="n">
-        <v>0.001825335581658998</v>
+        <v>0</v>
       </c>
       <c r="O30" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0</v>
       </c>
       <c r="P30" t="n">
-        <v>1.905360732420665e-05</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="Q30" t="n">
         <v>0</v>
       </c>
       <c r="R30" t="n">
-        <v>0.002456009984090238</v>
+        <v>1.544715088335636e-05</v>
       </c>
       <c r="S30" t="n">
-        <v>0.01281926700772624</v>
+        <v>0.0004943088282674034</v>
       </c>
       <c r="T30" t="n">
-        <v>0.0024617260662875</v>
+        <v>0</v>
       </c>
       <c r="U30" t="n">
-        <v>0</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="V30" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="W30" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>1.324041504287688e-05</v>
       </c>
       <c r="X30" t="n">
-        <v>0.006855487915249554</v>
+        <v>0.001235772070668509</v>
       </c>
       <c r="Y30" t="n">
-        <v>0.0008802766583783474</v>
+        <v>0</v>
       </c>
       <c r="Z30" t="n">
         <v>0</v>
       </c>
       <c r="AA30" t="n">
-        <v>5.906618270504063e-05</v>
+        <v>0</v>
       </c>
       <c r="AB30" t="n">
         <v>0</v>
       </c>
       <c r="AC30" t="n">
-        <v>0.00183105166385626</v>
+        <v>0</v>
       </c>
       <c r="AD30" t="n">
-        <v>1.333752512694466e-05</v>
+        <v>0</v>
       </c>
       <c r="AE30" t="n">
         <v>0</v>
       </c>
       <c r="AF30" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AG30" t="n">
-        <v>0</v>
+        <v>0.00195075448298386</v>
       </c>
       <c r="AH30" t="n">
-        <v>0</v>
+        <v>0.0003508709986362373</v>
       </c>
     </row>
     <row r="31">
@@ -3681,76 +3681,76 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1.333752512694466e-05</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0003791667857517125</v>
+        <v>0.0007282228273582283</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>3.31010376071922e-05</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>4.95393790429373e-05</v>
+        <v>0</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="L31" t="n">
         <v>0</v>
       </c>
       <c r="M31" t="n">
-        <v>0.0006725923385444949</v>
+        <v>0</v>
       </c>
       <c r="N31" t="n">
-        <v>4.572865757809597e-05</v>
+        <v>0</v>
       </c>
       <c r="O31" t="n">
-        <v>2.286432878904799e-05</v>
+        <v>0</v>
       </c>
       <c r="P31" t="n">
-        <v>0.0006459172882906057</v>
+        <v>0</v>
       </c>
       <c r="Q31" t="n">
-        <v>0.0001314698905370259</v>
+        <v>0</v>
       </c>
       <c r="R31" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="S31" t="n">
-        <v>0.005516019320357827</v>
+        <v>0</v>
       </c>
       <c r="T31" t="n">
-        <v>0.001028894795507159</v>
+        <v>0</v>
       </c>
       <c r="U31" t="n">
         <v>0</v>
       </c>
       <c r="V31" t="n">
-        <v>0.0004058418360056018</v>
+        <v>1.324041504287688e-05</v>
       </c>
       <c r="W31" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="X31" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="Y31" t="n">
-        <v>0.001084150256747359</v>
+        <v>0</v>
       </c>
       <c r="Z31" t="n">
         <v>0</v>
@@ -3759,16 +3759,16 @@
         <v>0</v>
       </c>
       <c r="AB31" t="n">
-        <v>2.858041098630998e-05</v>
+        <v>0</v>
       </c>
       <c r="AC31" t="n">
         <v>0</v>
       </c>
       <c r="AD31" t="n">
-        <v>0.0003543970962302438</v>
+        <v>0</v>
       </c>
       <c r="AE31" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0</v>
       </c>
       <c r="AF31" t="n">
         <v>0</v>
@@ -3790,100 +3790,100 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0003239113245115131</v>
+        <v>8.826943361917918e-06</v>
       </c>
       <c r="D32" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>5.737513185246647e-05</v>
       </c>
       <c r="E32" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>0.0003045295459861682</v>
       </c>
       <c r="G32" t="n">
-        <v>8.764659369135062e-05</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>0.0001981575161717492</v>
+        <v>0</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>0.00320481675193156</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="K32" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.0001677119238764405</v>
       </c>
       <c r="L32" t="n">
-        <v>0.0004915830689645318</v>
+        <v>0</v>
       </c>
       <c r="M32" t="n">
-        <v>0.0004591919365133804</v>
+        <v>0</v>
       </c>
       <c r="N32" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0</v>
       </c>
       <c r="O32" t="n">
-        <v>0.0001371859727342879</v>
+        <v>0</v>
       </c>
       <c r="P32" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.007474214291703998</v>
       </c>
       <c r="Q32" t="n">
-        <v>0.0002210218449607972</v>
+        <v>6.620207521438439e-06</v>
       </c>
       <c r="R32" t="n">
-        <v>3.429649318357198e-05</v>
+        <v>0.0005009290357888418</v>
       </c>
       <c r="S32" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="T32" t="n">
-        <v>0</v>
+        <v>1.10336792023974e-05</v>
       </c>
       <c r="U32" t="n">
-        <v>0.000621147598769137</v>
+        <v>0.0002890823951028118</v>
       </c>
       <c r="V32" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0.000966550298130012</v>
       </c>
       <c r="W32" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.005015910565409857</v>
       </c>
       <c r="X32" t="n">
-        <v>5.716082197261997e-06</v>
+        <v>0</v>
       </c>
       <c r="Y32" t="n">
         <v>0</v>
       </c>
       <c r="Z32" t="n">
-        <v>0.0003391542103708785</v>
+        <v>0</v>
       </c>
       <c r="AA32" t="n">
-        <v>9.526803662103327e-06</v>
+        <v>0</v>
       </c>
       <c r="AB32" t="n">
-        <v>0</v>
+        <v>9.268290530013814e-05</v>
       </c>
       <c r="AC32" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.0003729383570410321</v>
       </c>
       <c r="AD32" t="n">
-        <v>0</v>
+        <v>9.047616945965866e-05</v>
       </c>
       <c r="AE32" t="n">
-        <v>0.0004210847218649671</v>
+        <v>0</v>
       </c>
       <c r="AF32" t="n">
         <v>0</v>
       </c>
       <c r="AG32" t="n">
-        <v>0.0001314698905370259</v>
+        <v>0</v>
       </c>
       <c r="AH32" t="n">
-        <v>0.0004020311145407604</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -3893,25 +3893,25 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.001760975200702625</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>6.620207521438439e-06</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0008288319186029895</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>0.0001886307125096459</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="F33" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>1.10336792023974e-05</v>
       </c>
       <c r="G33" t="n">
-        <v>1.333752512694466e-05</v>
+        <v>0.000156678244674043</v>
       </c>
       <c r="H33" t="n">
-        <v>0.0005792296626558823</v>
+        <v>0</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
@@ -3920,55 +3920,55 @@
         <v>0</v>
       </c>
       <c r="K33" t="n">
-        <v>0</v>
+        <v>8.826943361917918e-06</v>
       </c>
       <c r="L33" t="n">
-        <v>1.143216439452399e-05</v>
+        <v>0.0009488964114061762</v>
       </c>
       <c r="M33" t="n">
-        <v>0.001385197252469824</v>
+        <v>0</v>
       </c>
       <c r="N33" t="n">
-        <v>0.0001771985481151219</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="O33" t="n">
-        <v>1.905360732420665e-05</v>
+        <v>0</v>
       </c>
       <c r="P33" t="n">
-        <v>0.0002476968952146865</v>
+        <v>0.000966550298130012</v>
       </c>
       <c r="Q33" t="n">
-        <v>0</v>
+        <v>1.10336792023974e-05</v>
       </c>
       <c r="R33" t="n">
-        <v>0.0001009841188182953</v>
+        <v>0.0001147502637049329</v>
       </c>
       <c r="S33" t="n">
-        <v>0.001185134375565654</v>
+        <v>0.000105923320343015</v>
       </c>
       <c r="T33" t="n">
-        <v>0.00443758514580773</v>
+        <v>0</v>
       </c>
       <c r="U33" t="n">
-        <v>0.001335657873426886</v>
+        <v>1.986062256431532e-05</v>
       </c>
       <c r="V33" t="n">
-        <v>0.004731010698600512</v>
+        <v>4.192798096911011e-05</v>
       </c>
       <c r="W33" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="X33" t="n">
-        <v>0</v>
+        <v>0.002217769519681877</v>
       </c>
       <c r="Y33" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0</v>
       </c>
       <c r="Z33" t="n">
         <v>0</v>
       </c>
       <c r="AA33" t="n">
-        <v>4.382329684567531e-05</v>
+        <v>0</v>
       </c>
       <c r="AB33" t="n">
         <v>0</v>
@@ -3977,19 +3977,19 @@
         <v>0</v>
       </c>
       <c r="AD33" t="n">
-        <v>1.905360732420666e-06</v>
+        <v>0</v>
       </c>
       <c r="AE33" t="n">
         <v>0</v>
       </c>
       <c r="AF33" t="n">
-        <v>0</v>
+        <v>0.0004236932813720601</v>
       </c>
       <c r="AG33" t="n">
-        <v>0.005666542818219059</v>
+        <v>3.31010376071922e-05</v>
       </c>
       <c r="AH33" t="n">
-        <v>0.0001486181371288119</v>
+        <v>0.0006333331862176106</v>
       </c>
     </row>
     <row r="34">
@@ -3999,85 +3999,85 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>2.667505025388932e-05</v>
+        <v>0.001725667427254953</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>0.000165505188035961</v>
       </c>
       <c r="D34" t="n">
-        <v>0.000621147598769137</v>
+        <v>0.0008694539211489149</v>
       </c>
       <c r="E34" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>6.620207521438439e-06</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>0.0002934958667837708</v>
       </c>
       <c r="G34" t="n">
-        <v>0.0001314698905370259</v>
+        <v>0.001255632693232824</v>
       </c>
       <c r="H34" t="n">
-        <v>0.0005030152333590557</v>
+        <v>0</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>0.0001314698905370259</v>
+        <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>0.0001028894795507159</v>
+        <v>0.000105923320343015</v>
       </c>
       <c r="L34" t="n">
-        <v>3.810721464841331e-06</v>
+        <v>0.007145410651472555</v>
       </c>
       <c r="M34" t="n">
-        <v>0.00340678498956815</v>
+        <v>8.164922609774074e-05</v>
       </c>
       <c r="N34" t="n">
-        <v>0.0003829775072165538</v>
+        <v>6.620207521438439e-05</v>
       </c>
       <c r="O34" t="n">
-        <v>3.239113245115131e-05</v>
+        <v>2.427409424527428e-05</v>
       </c>
       <c r="P34" t="n">
-        <v>0.007406137166919127</v>
+        <v>0.0028819970076662</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.0003429649318357198</v>
+        <v>0.000428106753053019</v>
       </c>
       <c r="R34" t="n">
-        <v>5.52554612401993e-05</v>
+        <v>0.0009555166189276147</v>
       </c>
       <c r="S34" t="n">
-        <v>0</v>
+        <v>0.000754703657443982</v>
       </c>
       <c r="T34" t="n">
-        <v>0.001295645298046052</v>
+        <v>5.737513185246647e-05</v>
       </c>
       <c r="U34" t="n">
-        <v>0</v>
+        <v>0.0006664342238248028</v>
       </c>
       <c r="V34" t="n">
-        <v>0.001615745901092724</v>
+        <v>0.004526015208823413</v>
       </c>
       <c r="W34" t="n">
-        <v>0.002101612887859994</v>
+        <v>0.0003442507911147988</v>
       </c>
       <c r="X34" t="n">
-        <v>7.621442929682663e-06</v>
+        <v>0.0001125435278644535</v>
       </c>
       <c r="Y34" t="n">
-        <v>0.0009183838730267607</v>
+        <v>0</v>
       </c>
       <c r="Z34" t="n">
-        <v>0</v>
+        <v>7.944249025726126e-05</v>
       </c>
       <c r="AA34" t="n">
-        <v>0</v>
+        <v>2.206735840479479e-06</v>
       </c>
       <c r="AB34" t="n">
-        <v>0.001619556622557566</v>
+        <v>0</v>
       </c>
       <c r="AC34" t="n">
         <v>0</v>
@@ -4086,16 +4086,16 @@
         <v>0</v>
       </c>
       <c r="AE34" t="n">
-        <v>0</v>
+        <v>0.0001986062256431532</v>
       </c>
       <c r="AF34" t="n">
-        <v>0</v>
+        <v>0.0001919860181217147</v>
       </c>
       <c r="AG34" t="n">
-        <v>0</v>
+        <v>4.413471680958959e-06</v>
       </c>
       <c r="AH34" t="n">
-        <v>0.002328350815018053</v>
+        <v>0.0002030196973241121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>